<commit_message>
Changed the village elders excel file
</commit_message>
<xml_diff>
--- a/Village Elders_id.xlsx
+++ b/Village Elders_id.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentsrwthaachende-my.sharepoint.com/personal/ycfr5qm97rgxxyet_students_rwth-aachen_de/Documents/Hiwi Job/OUI_Scrape_new/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="11_F25DC773A252ABDACC1048DDF11F73125ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F2C363D-5956-4734-84CD-CEFC57907339}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="11_F25DC773A252ABDACC1048DDF11F73125ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{149B4087-774E-4A0A-B8D2-AFBD78DAFF67}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2198,7 +2198,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2235,7 +2235,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>55660022100</v>
+        <v>15822422700</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2246,7 +2246,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>15822422700</v>
+        <v>55660022100</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2279,7 +2279,7 @@
         <v>14</v>
       </c>
       <c r="C7">
-        <v>8518796300</v>
+        <v>57607067000</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -2290,7 +2290,7 @@
         <v>14</v>
       </c>
       <c r="C8">
-        <v>57607067000</v>
+        <v>8518796300</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>